<commit_message>
Improve bathtub matching and add detailed logging for debugging
Adds debug logs and a second bathtub test case to bathtub_compatibility.py and test_compatibility.py, updates test data in test_bathtubs.py.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 0646a5b4-ba54-4146-8119-cc31c948a5ea
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/873c23c0-c18f-4e09-9f8d-38c5cb319996/d7fd3b02-2cbb-452d-b093-82b9fe7686f9.jpg
</commit_message>
<xml_diff>
--- a/data/test/test_product_data.xlsx
+++ b/data/test/test_product_data.xlsx
@@ -588,12 +588,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Maax</t>
+          <t>Swan</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Collection</t>
+          <t>Retail</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -800,7 +800,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -974,6 +974,58 @@
         <v>1200</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>WLL-003</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Test Alcove Tub Wall Kit Maax</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>60 x 32</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>60</v>
+      </c>
+      <c r="F4" t="n">
+        <v>32</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Alcove Tub Wall Kit</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Maax</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>MAAX</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Utile</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>950</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve the matching algorithm with more accurate test data
Updates test data path and fixes 'Series' name in test_bathtubs.py and test_compatibility.py.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 0646a5b4-ba54-4146-8119-cc31c948a5ea
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/873c23c0-c18f-4e09-9f8d-38c5cb319996/eb2e350a-a9a3-4de0-b0a9-8bdea8c98347.jpg
</commit_message>
<xml_diff>
--- a/data/test/test_product_data.xlsx
+++ b/data/test/test_product_data.xlsx
@@ -593,7 +593,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Retail</t>
+          <t>Swan</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -962,7 +962,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Retail</t>
+          <t>Swan</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">

</xml_diff>